<commit_message>
added more design changes and added requirements.txt
</commit_message>
<xml_diff>
--- a/data/Pokemon.xlsx
+++ b/data/Pokemon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Python\projects\data analysis\pokemon-stats-distribution\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A45E4B0-E507-4A03-A2DB-BA7C81E5615B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{036B48CC-66D3-4787-993C-D1E22EE57E96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{AB72914F-D51A-4499-ACEE-EF1BF01211EE}"/>
   </bookViews>
@@ -2928,6 +2928,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CBD9D367-30F9-4AFB-A80D-2BB03AB9870E}" name="Table1" displayName="Table1" ref="A1:M753" totalsRowShown="0">
   <autoFilter ref="A1:M753" xr:uid="{CBD9D367-30F9-4AFB-A80D-2BB03AB9870E}">
+    <filterColumn colId="3">
+      <filters blank="1"/>
+    </filterColumn>
     <filterColumn colId="12">
       <filters>
         <filter val="FALSE"/>
@@ -3273,10 +3276,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DCB0553-D5D7-4273-858F-8E7BF1CD667D}">
-  <dimension ref="A1:N753"/>
+  <dimension ref="A1:M753"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="A225" workbookViewId="0">
+      <selection activeCell="R254" sqref="R254"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3295,7 +3298,7 @@
     <col min="13" max="13" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3335,12 +3338,8 @@
       <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="str">
-        <f>IF(AND(ISNUMBER(SEARCH("Mega", B2)), NOT(OR(ISNUMBER(SEARCH("Yanmega", B2)), ISNUMBER(SEARCH("Meganium", B2)), ISNUMBER(SEARCH("Megahorn", B2))))), "Show", "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>289</v>
       </c>
@@ -3378,7 +3377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>149</v>
       </c>
@@ -3419,7 +3418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>151</v>
       </c>
@@ -3457,7 +3456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>248</v>
       </c>
@@ -3498,7 +3497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>251</v>
       </c>
@@ -3539,7 +3538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>373</v>
       </c>
@@ -3580,7 +3579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>376</v>
       </c>
@@ -3621,7 +3620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>445</v>
       </c>
@@ -3662,7 +3661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>488</v>
       </c>
@@ -3700,7 +3699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>490</v>
       </c>
@@ -3738,7 +3737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>635</v>
       </c>
@@ -3779,7 +3778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>648</v>
       </c>
@@ -3820,7 +3819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>648</v>
       </c>
@@ -3861,7 +3860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>649</v>
       </c>
@@ -3902,7 +3901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>706</v>
       </c>
@@ -4022,7 +4021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>567</v>
       </c>
@@ -4139,7 +4138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>637</v>
       </c>
@@ -4180,7 +4179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>468</v>
       </c>
@@ -4221,7 +4220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>130</v>
       </c>
@@ -4300,7 +4299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>230</v>
       </c>
@@ -4493,7 +4492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>555</v>
       </c>
@@ -4572,7 +4571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>131</v>
       </c>
@@ -4613,7 +4612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>169</v>
       </c>
@@ -4654,7 +4653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>260</v>
       </c>
@@ -4695,7 +4694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>462</v>
       </c>
@@ -4736,7 +4735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>464</v>
       </c>
@@ -4891,7 +4890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>715</v>
       </c>
@@ -4932,7 +4931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>6</v>
       </c>
@@ -5011,7 +5010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>392</v>
       </c>
@@ -5052,7 +5051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>655</v>
       </c>
@@ -5245,7 +5244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>257</v>
       </c>
@@ -5286,7 +5285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>306</v>
       </c>
@@ -5327,7 +5326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>365</v>
       </c>
@@ -5368,7 +5367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>395</v>
       </c>
@@ -5409,7 +5408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>473</v>
       </c>
@@ -5450,7 +5449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>652</v>
       </c>
@@ -5491,7 +5490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>658</v>
       </c>
@@ -5570,7 +5569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>500</v>
       </c>
@@ -5649,7 +5648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>3</v>
       </c>
@@ -5690,7 +5689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>91</v>
       </c>
@@ -5959,7 +5958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>389</v>
       </c>
@@ -6000,7 +5999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>448</v>
       </c>
@@ -6155,7 +6154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>476</v>
       </c>
@@ -6310,7 +6309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>697</v>
       </c>
@@ -6351,7 +6350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>699</v>
       </c>
@@ -6392,7 +6391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>103</v>
       </c>
@@ -6433,7 +6432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>121</v>
       </c>
@@ -6474,7 +6473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>330</v>
       </c>
@@ -6515,7 +6514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>479</v>
       </c>
@@ -6556,7 +6555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>479</v>
       </c>
@@ -6597,7 +6596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>479</v>
       </c>
@@ -6638,7 +6637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>479</v>
       </c>
@@ -6679,7 +6678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>479</v>
       </c>
@@ -6758,7 +6757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>609</v>
       </c>
@@ -6799,7 +6798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>681</v>
       </c>
@@ -6840,7 +6839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>681</v>
       </c>
@@ -6881,7 +6880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>553</v>
       </c>
@@ -6922,7 +6921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>282</v>
       </c>
@@ -6963,7 +6962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>475</v>
       </c>
@@ -7004,7 +7003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>73</v>
       </c>
@@ -7045,7 +7044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>142</v>
       </c>
@@ -7124,7 +7123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>407</v>
       </c>
@@ -7203,7 +7202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>469</v>
       </c>
@@ -7358,7 +7357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>62</v>
       </c>
@@ -7437,7 +7436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>208</v>
       </c>
@@ -7478,7 +7477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>461</v>
       </c>
@@ -7519,7 +7518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>472</v>
       </c>
@@ -7636,7 +7635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>628</v>
       </c>
@@ -7677,7 +7676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>630</v>
       </c>
@@ -7718,7 +7717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>537</v>
       </c>
@@ -7759,7 +7758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>530</v>
       </c>
@@ -7800,7 +7799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>668</v>
       </c>
@@ -7841,7 +7840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>31</v>
       </c>
@@ -7882,7 +7881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>34</v>
       </c>
@@ -7999,7 +7998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>213</v>
       </c>
@@ -8040,7 +8039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>430</v>
       </c>
@@ -8271,7 +8270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>94</v>
       </c>
@@ -8312,7 +8311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>123</v>
       </c>
@@ -8429,7 +8428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>212</v>
       </c>
@@ -8470,7 +8469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>214</v>
       </c>
@@ -8549,7 +8548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>229</v>
       </c>
@@ -8666,7 +8665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>344</v>
       </c>
@@ -8707,7 +8706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>437</v>
       </c>
@@ -8748,7 +8747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>452</v>
       </c>
@@ -8827,7 +8826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>542</v>
       </c>
@@ -8868,7 +8867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>689</v>
       </c>
@@ -8947,7 +8946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>701</v>
       </c>
@@ -8988,7 +8987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>703</v>
       </c>
@@ -9152,7 +9151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>663</v>
       </c>
@@ -9193,7 +9192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>426</v>
       </c>
@@ -9424,7 +9423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>76</v>
       </c>
@@ -9503,7 +9502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>139</v>
       </c>
@@ -9544,7 +9543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>141</v>
       </c>
@@ -9585,7 +9584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>346</v>
       </c>
@@ -9626,7 +9625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>348</v>
       </c>
@@ -9705,7 +9704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>411</v>
       </c>
@@ -9822,7 +9821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>565</v>
       </c>
@@ -9863,7 +9862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>589</v>
       </c>
@@ -9942,7 +9941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>675</v>
       </c>
@@ -9983,7 +9982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>460</v>
       </c>
@@ -10024,7 +10023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>691</v>
       </c>
@@ -10065,7 +10064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>711</v>
       </c>
@@ -10106,7 +10105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>711</v>
       </c>
@@ -10147,7 +10146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>711</v>
       </c>
@@ -10188,7 +10187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>711</v>
       </c>
@@ -10229,7 +10228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>45</v>
       </c>
@@ -10270,7 +10269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>71</v>
       </c>
@@ -10311,7 +10310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>80</v>
       </c>
@@ -10542,7 +10541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>199</v>
       </c>
@@ -10659,7 +10658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>334</v>
       </c>
@@ -10700,7 +10699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>454</v>
       </c>
@@ -10741,7 +10740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>561</v>
       </c>
@@ -10858,7 +10857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>625</v>
       </c>
@@ -10937,7 +10936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>598</v>
       </c>
@@ -10978,7 +10977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>521</v>
       </c>
@@ -11019,7 +11018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>560</v>
       </c>
@@ -11136,7 +11135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>112</v>
       </c>
@@ -11253,7 +11252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>369</v>
       </c>
@@ -11294,7 +11293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>398</v>
       </c>
@@ -11335,7 +11334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>442</v>
       </c>
@@ -11376,7 +11375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>545</v>
       </c>
@@ -11607,7 +11606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>632</v>
       </c>
@@ -11762,7 +11761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>623</v>
       </c>
@@ -11841,7 +11840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>687</v>
       </c>
@@ -11882,7 +11881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>695</v>
       </c>
@@ -11999,7 +11998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>272</v>
       </c>
@@ -12040,7 +12039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>275</v>
       </c>
@@ -12157,7 +12156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>478</v>
       </c>
@@ -12236,7 +12235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>547</v>
       </c>
@@ -12353,7 +12352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>593</v>
       </c>
@@ -12432,7 +12431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>18</v>
       </c>
@@ -12473,7 +12472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>435</v>
       </c>
@@ -12514,7 +12513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>87</v>
       </c>
@@ -12631,7 +12630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>332</v>
       </c>
@@ -12672,7 +12671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>423</v>
       </c>
@@ -12713,7 +12712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>558</v>
       </c>
@@ -12754,7 +12753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>586</v>
       </c>
@@ -12833,7 +12832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>416</v>
       </c>
@@ -12912,7 +12911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>709</v>
       </c>
@@ -13067,7 +13066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>581</v>
       </c>
@@ -13108,7 +13107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>596</v>
       </c>
@@ -13269,7 +13268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>618</v>
       </c>
@@ -13310,7 +13309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>178</v>
       </c>
@@ -13503,7 +13502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>707</v>
       </c>
@@ -13544,7 +13543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>340</v>
       </c>
@@ -13585,7 +13584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>342</v>
       </c>
@@ -13740,7 +13739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>82</v>
       </c>
@@ -13781,7 +13780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>205</v>
       </c>
@@ -13822,7 +13821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>226</v>
       </c>
@@ -13863,7 +13862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>227</v>
       </c>
@@ -14056,7 +14055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>591</v>
       </c>
@@ -14173,7 +14172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>85</v>
       </c>
@@ -14214,7 +14213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>122</v>
       </c>
@@ -14255,7 +14254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>171</v>
       </c>
@@ -14296,7 +14295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>189</v>
       </c>
@@ -14337,7 +14336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>286</v>
       </c>
@@ -14378,7 +14377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>319</v>
       </c>
@@ -14419,7 +14418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>323</v>
       </c>
@@ -14460,7 +14459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>357</v>
       </c>
@@ -14653,7 +14652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>291</v>
       </c>
@@ -14694,7 +14693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>42</v>
       </c>
@@ -14849,7 +14848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>124</v>
       </c>
@@ -14890,7 +14889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>203</v>
       </c>
@@ -15197,7 +15196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>49</v>
       </c>
@@ -15352,7 +15351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>221</v>
       </c>
@@ -15431,7 +15430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>680</v>
       </c>
@@ -15548,7 +15547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="310" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>22</v>
       </c>
@@ -15589,7 +15588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>164</v>
       </c>
@@ -15744,7 +15743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="315" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>337</v>
       </c>
@@ -15785,7 +15784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>338</v>
       </c>
@@ -15864,7 +15863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="318" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>479</v>
       </c>
@@ -15981,7 +15980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="321" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>40</v>
       </c>
@@ -16098,7 +16097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>702</v>
       </c>
@@ -16139,7 +16138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>195</v>
       </c>
@@ -16180,7 +16179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="326" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>207</v>
       </c>
@@ -16221,7 +16220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="327" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>211</v>
       </c>
@@ -16262,7 +16261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="328" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>215</v>
       </c>
@@ -16303,7 +16302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="329" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>277</v>
       </c>
@@ -16344,7 +16343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="330" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>279</v>
       </c>
@@ -16385,7 +16384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="331" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>305</v>
       </c>
@@ -16426,7 +16425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="332" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>587</v>
       </c>
@@ -16581,7 +16580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="336" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>528</v>
       </c>
@@ -16622,7 +16621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="337" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337">
         <v>413</v>
       </c>
@@ -16663,7 +16662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="338" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338">
         <v>413</v>
       </c>
@@ -16704,7 +16703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="339" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A339">
         <v>413</v>
       </c>
@@ -16745,7 +16744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="340" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A340">
         <v>414</v>
       </c>
@@ -16786,7 +16785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="341" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A341">
         <v>660</v>
       </c>
@@ -16865,7 +16864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="343" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A343">
         <v>184</v>
       </c>
@@ -17058,7 +17057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="348" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348">
         <v>375</v>
       </c>
@@ -17137,7 +17136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="350" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A350">
         <v>634</v>
       </c>
@@ -17178,7 +17177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="351" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A351">
         <v>499</v>
       </c>
@@ -17295,7 +17294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="354" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A354">
         <v>284</v>
       </c>
@@ -17450,7 +17449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="358" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A358">
         <v>441</v>
       </c>
@@ -17491,7 +17490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="359" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A359">
         <v>666</v>
       </c>
@@ -17608,7 +17607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="362" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A362">
         <v>219</v>
       </c>
@@ -17649,7 +17648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="363" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A363">
         <v>247</v>
       </c>
@@ -17690,7 +17689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="364" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A364">
         <v>308</v>
       </c>
@@ -17731,7 +17730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="365" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A365">
         <v>364</v>
       </c>
@@ -17772,7 +17771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="366" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A366">
         <v>400</v>
       </c>
@@ -17813,7 +17812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="367" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A367">
         <v>444</v>
       </c>
@@ -17930,7 +17929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="370" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A370">
         <v>2</v>
       </c>
@@ -18047,7 +18046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="373" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A373">
         <v>47</v>
       </c>
@@ -18164,7 +18163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="376" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A376">
         <v>93</v>
       </c>
@@ -18904,7 +18903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="395" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A395">
         <v>176</v>
       </c>
@@ -18945,7 +18944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="396" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A396">
         <v>198</v>
       </c>
@@ -19062,7 +19061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="399" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A399">
         <v>256</v>
       </c>
@@ -19103,7 +19102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="400" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A400">
         <v>259</v>
       </c>
@@ -19258,7 +19257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="404" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A404">
         <v>391</v>
       </c>
@@ -19527,7 +19526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="411" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A411">
         <v>566</v>
       </c>
@@ -19682,7 +19681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="415" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A415">
         <v>315</v>
       </c>
@@ -19761,7 +19760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="417" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A417">
         <v>12</v>
       </c>
@@ -19802,7 +19801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="418" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A418">
         <v>15</v>
       </c>
@@ -19843,7 +19842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="419" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A419">
         <v>44</v>
       </c>
@@ -19922,7 +19921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="421" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A421">
         <v>267</v>
       </c>
@@ -20001,7 +20000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="423" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A423">
         <v>70</v>
       </c>
@@ -20042,7 +20041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="424" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A424">
         <v>75</v>
       </c>
@@ -20083,7 +20082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="425" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A425">
         <v>166</v>
       </c>
@@ -20124,7 +20123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="426" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A426">
         <v>168</v>
       </c>
@@ -20165,7 +20164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="427" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A427">
         <v>193</v>
       </c>
@@ -20358,7 +20357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="432" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A432">
         <v>95</v>
       </c>
@@ -20437,7 +20436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="434" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A434">
         <v>269</v>
       </c>
@@ -20516,7 +20515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="436" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A436">
         <v>536</v>
       </c>
@@ -20557,7 +20556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="437" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A437">
         <v>662</v>
       </c>
@@ -20598,7 +20597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="438" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A438">
         <v>222</v>
       </c>
@@ -20677,7 +20676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="440" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A440">
         <v>302</v>
       </c>
@@ -20718,7 +20717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="441" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A441">
         <v>303</v>
       </c>
@@ -20759,7 +20758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="442" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A442">
         <v>541</v>
       </c>
@@ -20952,7 +20951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="447" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A447">
         <v>608</v>
       </c>
@@ -20993,7 +20992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="448" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A448">
         <v>629</v>
       </c>
@@ -21034,7 +21033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="449" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A449">
         <v>667</v>
       </c>
@@ -21265,7 +21264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="455" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A455">
         <v>696</v>
       </c>
@@ -21306,7 +21305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="456" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A456">
         <v>698</v>
       </c>
@@ -21499,7 +21498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="461" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A461">
         <v>544</v>
       </c>
@@ -21540,7 +21539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="462" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A462">
         <v>636</v>
       </c>
@@ -21581,7 +21580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="463" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A463">
         <v>520</v>
       </c>
@@ -21622,7 +21621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="464" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A464">
         <v>138</v>
       </c>
@@ -21663,7 +21662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="465" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A465">
         <v>140</v>
       </c>
@@ -21704,7 +21703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="466" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A466">
         <v>345</v>
       </c>
@@ -21745,7 +21744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="467" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A467">
         <v>347</v>
       </c>
@@ -21786,7 +21785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="468" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A468">
         <v>564</v>
       </c>
@@ -21865,7 +21864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="470" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A470">
         <v>83</v>
       </c>
@@ -21906,7 +21905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="471" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A471">
         <v>552</v>
       </c>
@@ -22023,7 +22022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="474" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A474">
         <v>410</v>
       </c>
@@ -22140,7 +22139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="477" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A477">
         <v>627</v>
       </c>
@@ -22219,7 +22218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="479" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A479">
         <v>17</v>
       </c>
@@ -22260,7 +22259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="480" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A480">
         <v>425</v>
       </c>
@@ -22301,7 +22300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="481" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A481">
         <v>559</v>
       </c>
@@ -22380,7 +22379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="483" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A483">
         <v>111</v>
       </c>
@@ -22459,7 +22458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="485" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A485">
         <v>458</v>
       </c>
@@ -22652,7 +22651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="490" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A490">
         <v>188</v>
       </c>
@@ -22693,7 +22692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="491" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A491">
         <v>271</v>
       </c>
@@ -22734,7 +22733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="492" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A492">
         <v>274</v>
       </c>
@@ -23132,7 +23131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="502" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="502" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A502">
         <v>329</v>
       </c>
@@ -23173,7 +23172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="503" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="503" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A503">
         <v>397</v>
       </c>
@@ -23214,7 +23213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="504" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="504" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A504">
         <v>624</v>
       </c>
@@ -23489,7 +23488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="511" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="511" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A511">
         <v>72</v>
       </c>
@@ -23568,7 +23567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="513" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="513" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A513">
         <v>585</v>
       </c>
@@ -23609,7 +23608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="514" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="514" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A514">
         <v>592</v>
       </c>
@@ -23688,7 +23687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="516" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="516" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A516">
         <v>710</v>
       </c>
@@ -23729,7 +23728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="517" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="517" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A517">
         <v>710</v>
       </c>
@@ -23770,7 +23769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="518" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="518" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A518">
         <v>710</v>
       </c>
@@ -23811,7 +23810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="519" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="519" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A519">
         <v>710</v>
       </c>
@@ -23852,7 +23851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="520" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="520" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A520">
         <v>459</v>
       </c>
@@ -23931,7 +23930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="522" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="522" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A522">
         <v>170</v>
       </c>
@@ -24010,7 +24009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="524" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="524" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A524">
         <v>225</v>
       </c>
@@ -24051,7 +24050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="525" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="525" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A525">
         <v>228</v>
       </c>
@@ -24130,7 +24129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="527" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="527" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A527">
         <v>304</v>
       </c>
@@ -24323,7 +24322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="532" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="532" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A532">
         <v>451</v>
       </c>
@@ -24478,7 +24477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="536" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="536" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A536">
         <v>434</v>
       </c>
@@ -24633,7 +24632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="540" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="540" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A540">
         <v>81</v>
       </c>
@@ -24788,7 +24787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="544" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="544" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A544">
         <v>102</v>
       </c>
@@ -24905,7 +24904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="547" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="547" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A547">
         <v>557</v>
       </c>
@@ -24946,7 +24945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="548" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="548" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A548">
         <v>679</v>
       </c>
@@ -25063,7 +25062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="551" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="551" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A551">
         <v>43</v>
       </c>
@@ -25218,7 +25217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="555" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="555" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A555">
         <v>177</v>
       </c>
@@ -25297,7 +25296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="557" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="557" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A557">
         <v>690</v>
       </c>
@@ -25338,7 +25337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="558" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="558" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A558">
         <v>595</v>
       </c>
@@ -25379,7 +25378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="559" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="559" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A559">
         <v>1</v>
       </c>
@@ -25610,7 +25609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="565" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="565" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A565">
         <v>79</v>
       </c>
@@ -25879,7 +25878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="572" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="572" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A572">
         <v>527</v>
       </c>
@@ -25996,7 +25995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="575" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="575" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A575">
         <v>84</v>
       </c>
@@ -26037,7 +26036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="576" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="576" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A576">
         <v>92</v>
       </c>
@@ -26192,7 +26191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="580" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="580" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A580">
         <v>333</v>
       </c>
@@ -26271,7 +26270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="582" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="582" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A582">
         <v>439</v>
       </c>
@@ -26312,7 +26311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="583" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="583" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A583">
         <v>540</v>
       </c>
@@ -26467,7 +26466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="587" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="587" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A587">
         <v>708</v>
       </c>
@@ -26698,7 +26697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="593" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="593" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A593">
         <v>688</v>
       </c>
@@ -26739,7 +26738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="594" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="594" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A594">
         <v>48</v>
       </c>
@@ -26894,7 +26893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="598" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="598" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A598">
         <v>238</v>
       </c>
@@ -26935,7 +26934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="599" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="599" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A599">
         <v>318</v>
       </c>
@@ -26976,7 +26975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="600" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="600" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A600">
         <v>322</v>
       </c>
@@ -27055,7 +27054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="602" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="602" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A602">
         <v>580</v>
       </c>
@@ -27134,7 +27133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="604" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="604" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A604">
         <v>597</v>
       </c>
@@ -27327,7 +27326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="609" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="609" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A609">
         <v>622</v>
       </c>
@@ -27520,7 +27519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="614" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="614" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A614">
         <v>69</v>
       </c>
@@ -27561,7 +27560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="615" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="615" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A615">
         <v>74</v>
       </c>
@@ -27716,7 +27715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="619" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="619" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A619">
         <v>246</v>
       </c>
@@ -27757,7 +27756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="620" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="620" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A620">
         <v>343</v>
       </c>
@@ -27874,7 +27873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="623" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="623" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A623">
         <v>374</v>
       </c>
@@ -27915,7 +27914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="624" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="624" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A624">
         <v>436</v>
       </c>
@@ -27956,7 +27955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="625" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="625" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A625">
         <v>443</v>
       </c>
@@ -27997,7 +27996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="626" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="626" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A626">
         <v>453</v>
       </c>
@@ -28114,7 +28113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="629" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="629" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A629">
         <v>633</v>
       </c>
@@ -28497,7 +28496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="639" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="639" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A639">
         <v>590</v>
       </c>
@@ -28576,7 +28575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="641" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="641" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A641">
         <v>551</v>
       </c>
@@ -28731,7 +28730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="645" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="645" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A645">
         <v>363</v>
       </c>
@@ -28886,7 +28885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="649" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="649" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A649">
         <v>694</v>
       </c>
@@ -29003,7 +29002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="652" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="652" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A652">
         <v>339</v>
       </c>
@@ -29044,7 +29043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="653" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="653" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A653">
         <v>686</v>
       </c>
@@ -29653,7 +29652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="668" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="668" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A668">
         <v>46</v>
       </c>
@@ -29884,7 +29883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="674" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="674" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A674">
         <v>307</v>
       </c>
@@ -29925,7 +29924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="675" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="675" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A675">
         <v>406</v>
       </c>
@@ -30004,7 +30003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="677" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="677" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A677">
         <v>546</v>
       </c>
@@ -30083,7 +30082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="679" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="679" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A679">
         <v>281</v>
       </c>
@@ -30124,7 +30123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="680" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="680" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A680">
         <v>661</v>
       </c>
@@ -30317,7 +30316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="685" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="685" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A685">
         <v>607</v>
       </c>
@@ -30396,7 +30395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="687" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="687" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A687">
         <v>39</v>
       </c>
@@ -30437,7 +30436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="688" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="688" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A688">
         <v>276</v>
       </c>
@@ -30478,7 +30477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="689" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="689" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A689">
         <v>278</v>
       </c>
@@ -30519,7 +30518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="690" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="690" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A690">
         <v>283</v>
       </c>
@@ -30560,7 +30559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="691" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="691" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A691">
         <v>290</v>
       </c>
@@ -30639,7 +30638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="693" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="693" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A693">
         <v>165</v>
       </c>
@@ -30680,7 +30679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="694" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="694" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A694">
         <v>519</v>
       </c>
@@ -30759,7 +30758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="696" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="696" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A696">
         <v>21</v>
       </c>
@@ -30800,7 +30799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="697" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="697" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A697">
         <v>163</v>
       </c>
@@ -30917,7 +30916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="700" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="700" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A700">
         <v>543</v>
       </c>
@@ -31034,7 +31033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="703" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="703" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A703">
         <v>16</v>
       </c>
@@ -31075,7 +31074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="704" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="704" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A704">
         <v>167</v>
       </c>
@@ -31116,7 +31115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="705" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="705" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A705">
         <v>183</v>
       </c>
@@ -31157,7 +31156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="706" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="706" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A706">
         <v>187</v>
       </c>
@@ -31236,7 +31235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="708" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="708" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A708">
         <v>220</v>
       </c>
@@ -31353,7 +31352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="711" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="711" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A711">
         <v>41</v>
       </c>
@@ -31432,7 +31431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="713" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="713" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A713">
         <v>396</v>
       </c>
@@ -31473,7 +31472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="714" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="714" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A714">
         <v>714</v>
       </c>
@@ -31514,7 +31513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="715" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="715" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A715">
         <v>415</v>
       </c>
@@ -31707,7 +31706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="720" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="720" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A720">
         <v>292</v>
       </c>
@@ -31824,7 +31823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="723" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="723" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A723">
         <v>270</v>
       </c>
@@ -32055,7 +32054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="729" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="729" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A729">
         <v>174</v>
       </c>
@@ -32096,7 +32095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="730" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="730" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A730">
         <v>194</v>
       </c>
@@ -32213,7 +32212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="733" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="733" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A733">
         <v>14</v>
       </c>
@@ -32482,7 +32481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="740" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="740" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A740">
         <v>280</v>
       </c>
@@ -32561,7 +32560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="742" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="742" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A742">
         <v>13</v>
       </c>
@@ -32678,7 +32677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="745" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="745" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A745">
         <v>298</v>
       </c>

</xml_diff>